<commit_message>
Updated text notes and sourcing
</commit_message>
<xml_diff>
--- a/HBCU R3 to R2 data 20250128.xlsx
+++ b/HBCU R3 to R2 data 20250128.xlsx
@@ -8,23 +8,23 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/im436/Library/CloudStorage/GoogleDrive-im436@georgetown.edu/Shared drives/CSET/Analysis Team/Igor/For Jaret/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99DDC0A7-2F90-6741-8FCF-F270B27AA824}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{286F816B-DC74-764A-97E1-64EB50693554}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35360" yWindow="2080" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="33280" yWindow="1940" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Full Version" sheetId="2" r:id="rId1"/>
     <sheet name="Table for Export" sheetId="4" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Titles" localSheetId="0">'Full Version'!$6:$7</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="0">'Full Version'!$5:$6</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="49">
   <si>
     <t>Classification</t>
   </si>
@@ -131,61 +131,9 @@
     <t>Grambling State University</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Garamond, serif"/>
-      </rPr>
-      <t>Note: Table 1 below presents 2023 totals for research PhD conferrals (source: IPEDS, see Note below) and R&amp;D expenditure (source: HERD, see Note below) for the 29 research doctorate-granting HBCU institutions. The numbers in the parentheses represent the average for the past three years, 2023 - 2021. Note that starting in 2025 Carnegie will use the highest of these two numbers to determine research classification status. The Carnegie classifications are determined using data from the National Science Foundation (NSF) National Center for Science and Engineering Statistics (NCSES) Higher Education Research and Development (</t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="12"/>
-        <color rgb="FF1155CC"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>HERD</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Garamond, serif"/>
-      </rPr>
-      <t>) survey and the U.S. Department of Education Institute of Education Sciences National Center of Education Statistics Integrated Postsecondary Education System (</t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="12"/>
-        <color rgb="FF1155CC"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>IPEDS</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Garamond, serif"/>
-      </rPr>
-      <t xml:space="preserve">). </t>
-    </r>
-  </si>
-  <si>
-    <t>Table 1. Current R2 and “R3” (R2 aspiring) HBCUs (2023), with averages for prior three years (2023, 2022, and 2021)</t>
-  </si>
-  <si>
     <t>3 Year Average</t>
   </si>
   <si>
-    <t>Source: “Table Builder | NCSES | NSF.” https://ncsesdata.nsf.gov/builder/herd; National Center for Education Statistics, “IPEDS Integrated Postsecondary Education Data System: Custom Data Files.”</t>
-  </si>
-  <si>
     <t>Alabama A&amp;M University</t>
   </si>
   <si>
@@ -208,6 +156,25 @@
   </si>
   <si>
     <t>R3 Group 3</t>
+  </si>
+  <si>
+    <t>Table 1 below presents 2023 totals for research Ph.D. conferrals and R&amp;D expenditure for the 29 research doctorate-granting HBCU institutions that are classified as R2 or potentially aspire to R2 classification under the Carnegie research classification system, as well as the average of these values over the past three years (2021 - 2023). Starting in 2025 Carnegie will use the highest of these two numbers (current total and 3-year average) when determining research classification status.
+The Carnegie classifications are determined using data from the National Science Foundation (NSF) National Center for Science and Engineering Statistics (NCSES) Higher Education Research and Development (HERD) survey and the U.S. Department of Education Institute of Education Sciences National Center of Education Statistics Integrated Postsecondary Education System (IPEDS).</t>
+  </si>
+  <si>
+    <t>Sources</t>
+  </si>
+  <si>
+    <t>Research Ph.D. conferrals are sourced from the National Center for Education Statistics, Integrated Postsecondary Education Data System (IPEDS)</t>
+  </si>
+  <si>
+    <t>R&amp;D expenditure data are sourced from the National Center for Science and Engineer Statistics' Higher Education Research and Development (HERD) Survey</t>
+  </si>
+  <si>
+    <t>The definition of STEM fields is sourced from the Department of Homeland Security's "Study in the States" which defines the list of degree programs that comprise STEM.</t>
+  </si>
+  <si>
+    <t>Table 1.  R2 and R2-aspiring (a.k.a., "R3") HBCUs as of 2023</t>
   </si>
 </sst>
 </file>
@@ -217,19 +184,12 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0"/>
   </numFmts>
-  <fonts count="16">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Garamond"/>
-      <family val="1"/>
     </font>
     <font>
       <b/>
@@ -256,18 +216,6 @@
       <color rgb="FF000000"/>
       <name val="Garamond"/>
       <family val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Garamond, serif"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="12"/>
-      <color rgb="FF1155CC"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
@@ -317,6 +265,15 @@
     <font>
       <sz val="8"/>
       <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -680,304 +637,312 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="104">
+  <cellXfs count="106">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="12" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="3" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="9" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="3" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="12" fillId="3" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="3" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="3" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="3" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="3" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="9" fillId="3" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="3" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="3" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="3" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="3" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="12" fillId="3" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="3" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="3" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="9" fillId="3" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="3" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="3" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="12" fillId="4" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="4" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="4" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="9" fillId="4" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="4" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="4" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="12" fillId="4" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="4" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="4" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="4" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="4" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="9" fillId="4" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="4" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="4" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="4" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="4" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="12" fillId="4" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="4" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="4" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="9" fillId="4" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="4" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="4" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="12" fillId="5" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="5" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="5" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="9" fillId="5" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="5" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="5" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="12" fillId="5" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="5" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="5" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="9" fillId="5" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="5" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="5" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="12" fillId="5" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="5" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="5" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="9" fillId="5" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="5" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="5" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="12" fillId="6" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="6" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="6" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="9" fillId="6" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="6" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="6" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="12" fillId="6" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="6" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="6" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="6" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="6" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="9" fillId="6" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="6" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="6" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="6" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="6" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="12" fillId="6" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="6" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="6" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="9" fillId="6" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="6" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="6" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="12" fillId="7" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="7" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="7" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="9" fillId="7" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="7" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="7" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="12" fillId="7" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="7" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="7" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="9" fillId="7" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="7" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="7" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="12" fillId="7" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="7" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="7" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="9" fillId="7" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="7" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="7" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1195,14 +1160,14 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A3:J38"/>
+  <dimension ref="A2:J41"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="7" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C37" sqref="C37"/>
+      <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="1.83203125" customWidth="1"/>
     <col min="2" max="2" width="17" customWidth="1"/>
@@ -1211,654 +1176,693 @@
     <col min="6" max="7" width="18.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:10" ht="104" customHeight="1">
-      <c r="A3" s="2"/>
-      <c r="B3" s="88" t="s">
+    <row r="2" spans="1:10" ht="134" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="2"/>
+      <c r="B2" s="103" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2" s="103"/>
+      <c r="D2" s="103"/>
+      <c r="E2" s="103"/>
+      <c r="F2" s="103"/>
+      <c r="G2" s="103"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+    </row>
+    <row r="4" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1"/>
+      <c r="B4" s="85" t="s">
+        <v>48</v>
+      </c>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+    </row>
+    <row r="5" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="3"/>
+      <c r="B5" s="99" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="101" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" s="97" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5" s="98"/>
+      <c r="F5" s="95" t="s">
+        <v>3</v>
+      </c>
+      <c r="G5" s="96"/>
+    </row>
+    <row r="6" spans="1:10" ht="36" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="3"/>
+      <c r="B6" s="100"/>
+      <c r="C6" s="102"/>
+      <c r="D6" s="11">
+        <v>2023</v>
+      </c>
+      <c r="E6" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="C3" s="88"/>
-      <c r="D3" s="88"/>
-      <c r="E3" s="88"/>
-      <c r="F3" s="88"/>
-      <c r="G3" s="88"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="5"/>
-      <c r="J3" s="5"/>
-    </row>
-    <row r="5" spans="1:10" ht="16" customHeight="1">
-      <c r="A5" s="1"/>
-      <c r="B5" s="85" t="s">
-        <v>35</v>
-      </c>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6"/>
-    </row>
-    <row r="6" spans="1:10" ht="33" customHeight="1">
-      <c r="A6" s="3"/>
-      <c r="B6" s="100" t="s">
-        <v>0</v>
-      </c>
-      <c r="C6" s="102" t="s">
-        <v>1</v>
-      </c>
-      <c r="D6" s="98" t="s">
-        <v>2</v>
-      </c>
-      <c r="E6" s="99"/>
-      <c r="F6" s="96" t="s">
-        <v>3</v>
-      </c>
-      <c r="G6" s="97"/>
-    </row>
-    <row r="7" spans="1:10" ht="36" customHeight="1">
-      <c r="A7" s="3"/>
-      <c r="B7" s="101"/>
-      <c r="C7" s="103"/>
-      <c r="D7" s="11">
+      <c r="F6" s="12">
         <v>2023</v>
       </c>
-      <c r="E7" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="F7" s="12">
-        <v>2023</v>
-      </c>
-      <c r="G7" s="13" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="42" customHeight="1">
+      <c r="G6" s="13" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="42" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A7" s="4"/>
+      <c r="B7" s="88" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="16">
+        <v>102</v>
+      </c>
+      <c r="E7" s="16">
+        <v>97</v>
+      </c>
+      <c r="F7" s="17">
+        <v>84756</v>
+      </c>
+      <c r="G7" s="18">
+        <v>68524</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="42" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="4"/>
-      <c r="B8" s="89" t="s">
-        <v>4</v>
-      </c>
-      <c r="C8" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="D8" s="16">
-        <v>102</v>
-      </c>
-      <c r="E8" s="16">
-        <v>97</v>
-      </c>
-      <c r="F8" s="17">
-        <v>84756</v>
-      </c>
-      <c r="G8" s="18">
-        <v>68524</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="42" customHeight="1">
+      <c r="B8" s="89"/>
+      <c r="C8" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="20">
+        <v>68</v>
+      </c>
+      <c r="E8" s="20">
+        <v>74</v>
+      </c>
+      <c r="F8" s="21">
+        <v>19457</v>
+      </c>
+      <c r="G8" s="22">
+        <v>17698</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="42" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="4"/>
-      <c r="B9" s="90"/>
+      <c r="B9" s="89"/>
       <c r="C9" s="19" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D9" s="20">
+        <v>59</v>
+      </c>
+      <c r="E9" s="20">
+        <v>67</v>
+      </c>
+      <c r="F9" s="21">
+        <v>43868</v>
+      </c>
+      <c r="G9" s="22">
+        <v>31326</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="42" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A10" s="4"/>
+      <c r="B10" s="89"/>
+      <c r="C10" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="20">
         <v>68</v>
-      </c>
-      <c r="E9" s="20">
-        <v>74</v>
-      </c>
-      <c r="F9" s="21">
-        <v>19457</v>
-      </c>
-      <c r="G9" s="22">
-        <v>17698</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="42" customHeight="1">
-      <c r="A10" s="4"/>
-      <c r="B10" s="90"/>
-      <c r="C10" s="19" t="s">
-        <v>7</v>
-      </c>
-      <c r="D10" s="20">
-        <v>59</v>
       </c>
       <c r="E10" s="20">
         <v>67</v>
       </c>
       <c r="F10" s="21">
-        <v>43868</v>
+        <v>62307</v>
       </c>
       <c r="G10" s="22">
-        <v>31326</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="42" customHeight="1">
+        <v>50322</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="42" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="4"/>
-      <c r="B11" s="90"/>
+      <c r="B11" s="89"/>
       <c r="C11" s="19" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D11" s="20">
-        <v>68</v>
+        <v>44</v>
       </c>
       <c r="E11" s="20">
-        <v>67</v>
-      </c>
-      <c r="F11" s="21">
-        <v>62307</v>
-      </c>
-      <c r="G11" s="22">
-        <v>50322</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="42" customHeight="1">
+        <v>45</v>
+      </c>
+      <c r="F11" s="23">
+        <v>28246</v>
+      </c>
+      <c r="G11" s="24">
+        <v>24379</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="42" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="4"/>
-      <c r="B12" s="90"/>
+      <c r="B12" s="89"/>
       <c r="C12" s="19" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D12" s="20">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="E12" s="20">
-        <v>45</v>
-      </c>
-      <c r="F12" s="23">
-        <v>28246</v>
-      </c>
-      <c r="G12" s="24">
-        <v>24379</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="42" customHeight="1">
+        <v>38</v>
+      </c>
+      <c r="F12" s="21">
+        <v>10320</v>
+      </c>
+      <c r="G12" s="22">
+        <v>9334</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="42" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="4"/>
-      <c r="B13" s="90"/>
+      <c r="B13" s="89"/>
       <c r="C13" s="19" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D13" s="20">
+        <v>33</v>
+      </c>
+      <c r="E13" s="20">
+        <v>31</v>
+      </c>
+      <c r="F13" s="21">
+        <v>65159</v>
+      </c>
+      <c r="G13" s="22">
+        <v>54306</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="42" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A14" s="4"/>
+      <c r="B14" s="89"/>
+      <c r="C14" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="D14" s="20">
+        <v>26</v>
+      </c>
+      <c r="E14" s="20">
+        <v>21</v>
+      </c>
+      <c r="F14" s="21">
+        <v>21791</v>
+      </c>
+      <c r="G14" s="22">
+        <v>19934</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="42" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A15" s="4"/>
+      <c r="B15" s="89"/>
+      <c r="C15" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="E13" s="20">
-        <v>38</v>
-      </c>
-      <c r="F13" s="21">
-        <v>10320</v>
-      </c>
-      <c r="G13" s="22">
-        <v>9334</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" ht="42" customHeight="1">
-      <c r="A14" s="4"/>
-      <c r="B14" s="90"/>
-      <c r="C14" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="D14" s="20">
-        <v>33</v>
-      </c>
-      <c r="E14" s="20">
-        <v>31</v>
-      </c>
-      <c r="F14" s="21">
-        <v>65159</v>
-      </c>
-      <c r="G14" s="22">
-        <v>54306</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" ht="42" customHeight="1">
-      <c r="A15" s="4"/>
-      <c r="B15" s="90"/>
-      <c r="C15" s="19" t="s">
-        <v>40</v>
-      </c>
       <c r="D15" s="20">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="E15" s="20">
-        <v>21</v>
-      </c>
-      <c r="F15" s="21">
-        <v>21791</v>
-      </c>
-      <c r="G15" s="22">
-        <v>19934</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" ht="42" customHeight="1">
+        <v>22</v>
+      </c>
+      <c r="F15" s="23">
+        <v>5201</v>
+      </c>
+      <c r="G15" s="24">
+        <v>5236</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="42" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="4"/>
-      <c r="B16" s="90"/>
+      <c r="B16" s="89"/>
       <c r="C16" s="19" t="s">
-        <v>39</v>
+        <v>12</v>
       </c>
       <c r="D16" s="20">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="E16" s="20">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="F16" s="23">
-        <v>5201</v>
+        <v>16287</v>
       </c>
       <c r="G16" s="24">
-        <v>5236</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="42" customHeight="1">
+        <v>12512</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="42" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="4"/>
       <c r="B17" s="90"/>
-      <c r="C17" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="D17" s="20">
+      <c r="C17" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="D17" s="26">
+        <v>16</v>
+      </c>
+      <c r="E17" s="26">
+        <v>18</v>
+      </c>
+      <c r="F17" s="27">
+        <v>10730</v>
+      </c>
+      <c r="G17" s="28">
+        <v>9547</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="42" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A18" s="4"/>
+      <c r="B18" s="91" t="s">
+        <v>38</v>
+      </c>
+      <c r="C18" s="30" t="s">
+        <v>14</v>
+      </c>
+      <c r="D18" s="31">
         <v>28</v>
       </c>
-      <c r="E17" s="20">
+      <c r="E18" s="31">
         <v>27</v>
       </c>
-      <c r="F17" s="23">
-        <v>16287</v>
-      </c>
-      <c r="G17" s="24">
-        <v>12512</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="42" customHeight="1">
-      <c r="A18" s="4"/>
-      <c r="B18" s="91"/>
-      <c r="C18" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="D18" s="26">
+      <c r="F18" s="32">
+        <v>9769</v>
+      </c>
+      <c r="G18" s="33">
+        <v>10967</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="42" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A19" s="4"/>
+      <c r="B19" s="89"/>
+      <c r="C19" s="34" t="s">
+        <v>15</v>
+      </c>
+      <c r="D19" s="35">
+        <v>27</v>
+      </c>
+      <c r="E19" s="35">
+        <v>15</v>
+      </c>
+      <c r="F19" s="36">
+        <v>13504</v>
+      </c>
+      <c r="G19" s="37">
+        <v>11984</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="42" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A20" s="4"/>
+      <c r="B20" s="89"/>
+      <c r="C20" s="34" t="s">
         <v>16</v>
       </c>
-      <c r="E18" s="26">
-        <v>18</v>
-      </c>
-      <c r="F18" s="27">
-        <v>10730</v>
-      </c>
-      <c r="G18" s="28">
-        <v>9547</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="42" customHeight="1">
-      <c r="A19" s="4"/>
-      <c r="B19" s="92" t="s">
-        <v>41</v>
-      </c>
-      <c r="C19" s="30" t="s">
-        <v>14</v>
-      </c>
-      <c r="D19" s="31">
-        <v>28</v>
-      </c>
-      <c r="E19" s="31">
-        <v>27</v>
-      </c>
-      <c r="F19" s="32">
-        <v>9769</v>
-      </c>
-      <c r="G19" s="33">
-        <v>10967</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="42" customHeight="1">
-      <c r="A20" s="4"/>
-      <c r="B20" s="90"/>
-      <c r="C20" s="34" t="s">
-        <v>15</v>
-      </c>
       <c r="D20" s="35">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E20" s="35">
-        <v>15</v>
-      </c>
-      <c r="F20" s="36">
-        <v>13504</v>
-      </c>
-      <c r="G20" s="37">
-        <v>11984</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" ht="42" customHeight="1">
+        <v>20</v>
+      </c>
+      <c r="F20" s="38">
+        <v>33499</v>
+      </c>
+      <c r="G20" s="39">
+        <v>28569</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="42" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="4"/>
       <c r="B21" s="90"/>
-      <c r="C21" s="34" t="s">
-        <v>16</v>
-      </c>
-      <c r="D21" s="35">
+      <c r="C21" s="40" t="s">
+        <v>17</v>
+      </c>
+      <c r="D21" s="41">
         <v>25</v>
       </c>
-      <c r="E21" s="35">
+      <c r="E21" s="41">
+        <v>19</v>
+      </c>
+      <c r="F21" s="42">
+        <v>7814</v>
+      </c>
+      <c r="G21" s="43">
+        <v>5339</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="42" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A22" s="4"/>
+      <c r="B22" s="92" t="s">
+        <v>18</v>
+      </c>
+      <c r="C22" s="45" t="s">
+        <v>19</v>
+      </c>
+      <c r="D22" s="46">
+        <v>13</v>
+      </c>
+      <c r="E22" s="46">
+        <v>9</v>
+      </c>
+      <c r="F22" s="47">
+        <v>20259</v>
+      </c>
+      <c r="G22" s="48">
+        <v>18583</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="42" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A23" s="4"/>
+      <c r="B23" s="89"/>
+      <c r="C23" s="49" t="s">
         <v>20</v>
       </c>
-      <c r="F21" s="38">
-        <v>33499</v>
-      </c>
-      <c r="G21" s="39">
-        <v>28569</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" ht="42" customHeight="1">
-      <c r="A22" s="4"/>
-      <c r="B22" s="91"/>
-      <c r="C22" s="40" t="s">
-        <v>17</v>
-      </c>
-      <c r="D22" s="41">
-        <v>25</v>
-      </c>
-      <c r="E22" s="41">
-        <v>19</v>
-      </c>
-      <c r="F22" s="42">
-        <v>7814</v>
-      </c>
-      <c r="G22" s="43">
-        <v>5339</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" ht="42" customHeight="1">
-      <c r="A23" s="4"/>
-      <c r="B23" s="93" t="s">
-        <v>18</v>
-      </c>
-      <c r="C23" s="45" t="s">
-        <v>19</v>
-      </c>
-      <c r="D23" s="46">
-        <v>13</v>
-      </c>
-      <c r="E23" s="46">
-        <v>9</v>
-      </c>
-      <c r="F23" s="47">
-        <v>20259</v>
-      </c>
-      <c r="G23" s="48">
-        <v>18583</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" ht="42" customHeight="1">
+      <c r="D23" s="50">
+        <v>11</v>
+      </c>
+      <c r="E23" s="50">
+        <v>8</v>
+      </c>
+      <c r="F23" s="51">
+        <v>25625</v>
+      </c>
+      <c r="G23" s="52">
+        <v>22974</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="42" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="4"/>
       <c r="B24" s="90"/>
-      <c r="C24" s="49" t="s">
-        <v>20</v>
-      </c>
-      <c r="D24" s="50">
-        <v>11</v>
-      </c>
-      <c r="E24" s="50">
+      <c r="C24" s="53" t="s">
+        <v>21</v>
+      </c>
+      <c r="D24" s="54">
+        <v>10</v>
+      </c>
+      <c r="E24" s="54">
+        <v>10</v>
+      </c>
+      <c r="F24" s="55">
+        <v>6194</v>
+      </c>
+      <c r="G24" s="56">
+        <v>4701</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="42" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A25" s="4"/>
+      <c r="B25" s="93" t="s">
+        <v>22</v>
+      </c>
+      <c r="C25" s="58" t="s">
+        <v>23</v>
+      </c>
+      <c r="D25" s="59">
         <v>8</v>
       </c>
-      <c r="F24" s="51">
-        <v>25625</v>
-      </c>
-      <c r="G24" s="52">
-        <v>22974</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" ht="42" customHeight="1">
-      <c r="A25" s="4"/>
-      <c r="B25" s="91"/>
-      <c r="C25" s="53" t="s">
-        <v>21</v>
-      </c>
-      <c r="D25" s="54">
-        <v>10</v>
-      </c>
-      <c r="E25" s="54">
-        <v>10</v>
-      </c>
-      <c r="F25" s="55">
-        <v>6194</v>
-      </c>
-      <c r="G25" s="56">
-        <v>4701</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" ht="42" customHeight="1">
+      <c r="E25" s="59">
+        <v>3</v>
+      </c>
+      <c r="F25" s="60">
+        <v>7945</v>
+      </c>
+      <c r="G25" s="61">
+        <v>8943</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="42" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="4"/>
-      <c r="B26" s="94" t="s">
-        <v>22</v>
-      </c>
-      <c r="C26" s="58" t="s">
-        <v>23</v>
-      </c>
-      <c r="D26" s="59">
-        <v>8</v>
-      </c>
-      <c r="E26" s="59">
-        <v>3</v>
-      </c>
-      <c r="F26" s="60">
-        <v>7945</v>
-      </c>
-      <c r="G26" s="61">
-        <v>8943</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" ht="42" customHeight="1">
+      <c r="B26" s="89"/>
+      <c r="C26" s="62" t="s">
+        <v>24</v>
+      </c>
+      <c r="D26" s="63">
+        <v>5</v>
+      </c>
+      <c r="E26" s="63">
+        <v>7</v>
+      </c>
+      <c r="F26" s="64">
+        <v>57125</v>
+      </c>
+      <c r="G26" s="65">
+        <v>44084</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="42" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="4"/>
-      <c r="B27" s="90"/>
+      <c r="B27" s="89"/>
       <c r="C27" s="62" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D27" s="63">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E27" s="63">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F27" s="64">
-        <v>57125</v>
+        <v>22002</v>
       </c>
       <c r="G27" s="65">
-        <v>44084</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" ht="42" customHeight="1">
+        <v>18583</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="42" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="4"/>
-      <c r="B28" s="90"/>
+      <c r="B28" s="89"/>
       <c r="C28" s="62" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D28" s="63">
         <v>6</v>
       </c>
       <c r="E28" s="63">
+        <v>5</v>
+      </c>
+      <c r="F28" s="66">
+        <v>15519</v>
+      </c>
+      <c r="G28" s="67">
+        <v>12593</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="42" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A29" s="4"/>
+      <c r="B29" s="89"/>
+      <c r="C29" s="62" t="s">
+        <v>35</v>
+      </c>
+      <c r="D29" s="63">
+        <v>3</v>
+      </c>
+      <c r="E29" s="63">
         <v>6</v>
       </c>
-      <c r="F28" s="64">
-        <v>22002</v>
-      </c>
-      <c r="G28" s="65">
-        <v>18583</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" ht="42" customHeight="1">
-      <c r="A29" s="4"/>
-      <c r="B29" s="90"/>
-      <c r="C29" s="62" t="s">
-        <v>26</v>
-      </c>
-      <c r="D29" s="63">
-        <v>6</v>
-      </c>
-      <c r="E29" s="63">
-        <v>5</v>
-      </c>
-      <c r="F29" s="66">
-        <v>15519</v>
-      </c>
-      <c r="G29" s="67">
-        <v>12593</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" ht="42" customHeight="1">
+      <c r="F29" s="64">
+        <v>15588</v>
+      </c>
+      <c r="G29" s="65">
+        <v>11460</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="42" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="4"/>
-      <c r="B30" s="90"/>
+      <c r="B30" s="89"/>
       <c r="C30" s="62" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="D30" s="63">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E30" s="63">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="F30" s="64">
-        <v>15588</v>
+        <v>18477</v>
       </c>
       <c r="G30" s="65">
-        <v>11460</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" ht="42" customHeight="1">
+        <v>16394</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="42" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="4"/>
       <c r="B31" s="90"/>
-      <c r="C31" s="62" t="s">
-        <v>27</v>
-      </c>
-      <c r="D31" s="63">
-        <v>2</v>
-      </c>
-      <c r="E31" s="63">
-        <v>1</v>
-      </c>
-      <c r="F31" s="64">
-        <v>18477</v>
-      </c>
-      <c r="G31" s="65">
-        <v>16394</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" ht="42" customHeight="1">
+      <c r="C31" s="68" t="s">
+        <v>28</v>
+      </c>
+      <c r="D31" s="69">
+        <v>0</v>
+      </c>
+      <c r="E31" s="69">
+        <v>0</v>
+      </c>
+      <c r="F31" s="70">
+        <v>7766</v>
+      </c>
+      <c r="G31" s="71">
+        <v>7995</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="42" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="4"/>
-      <c r="B32" s="91"/>
-      <c r="C32" s="68" t="s">
-        <v>28</v>
-      </c>
-      <c r="D32" s="69">
-        <v>0</v>
-      </c>
-      <c r="E32" s="69">
-        <v>0</v>
-      </c>
-      <c r="F32" s="70">
-        <v>7766</v>
-      </c>
-      <c r="G32" s="71">
-        <v>7995</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" ht="42" customHeight="1">
+      <c r="B32" s="94" t="s">
+        <v>29</v>
+      </c>
+      <c r="C32" s="73" t="s">
+        <v>30</v>
+      </c>
+      <c r="D32" s="74">
+        <v>17</v>
+      </c>
+      <c r="E32" s="74">
+        <v>13</v>
+      </c>
+      <c r="F32" s="75">
+        <v>2612</v>
+      </c>
+      <c r="G32" s="76">
+        <v>2454</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="42" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="4"/>
-      <c r="B33" s="95" t="s">
-        <v>29</v>
-      </c>
-      <c r="C33" s="73" t="s">
-        <v>30</v>
-      </c>
-      <c r="D33" s="74">
-        <v>17</v>
-      </c>
-      <c r="E33" s="74">
-        <v>13</v>
-      </c>
-      <c r="F33" s="75">
-        <v>2612</v>
-      </c>
-      <c r="G33" s="76">
-        <v>2454</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" ht="42" customHeight="1">
+      <c r="B33" s="89"/>
+      <c r="C33" s="77" t="s">
+        <v>31</v>
+      </c>
+      <c r="D33" s="78">
+        <v>15</v>
+      </c>
+      <c r="E33" s="78">
+        <v>16</v>
+      </c>
+      <c r="F33" s="79">
+        <v>3569</v>
+      </c>
+      <c r="G33" s="80">
+        <v>3569</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" ht="42" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="4"/>
-      <c r="B34" s="90"/>
+      <c r="B34" s="89"/>
       <c r="C34" s="77" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D34" s="78">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="E34" s="78">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="F34" s="79">
-        <v>3569</v>
+        <v>3229</v>
       </c>
       <c r="G34" s="80">
-        <v>3569</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" ht="42" customHeight="1">
+        <v>3013</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="42" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="4"/>
       <c r="B35" s="90"/>
-      <c r="C35" s="77" t="s">
-        <v>32</v>
-      </c>
-      <c r="D35" s="78">
-        <v>4</v>
-      </c>
-      <c r="E35" s="78">
-        <v>7</v>
-      </c>
-      <c r="F35" s="79">
-        <v>3229</v>
-      </c>
-      <c r="G35" s="80">
-        <v>3013</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" ht="42" customHeight="1">
-      <c r="A36" s="4"/>
-      <c r="B36" s="91"/>
-      <c r="C36" s="81" t="s">
+      <c r="C35" s="81" t="s">
         <v>33</v>
       </c>
-      <c r="D36" s="82">
+      <c r="D35" s="82">
         <v>2</v>
       </c>
-      <c r="E36" s="82">
+      <c r="E35" s="82">
         <v>5</v>
       </c>
-      <c r="F36" s="83">
+      <c r="F35" s="83">
         <v>449</v>
       </c>
-      <c r="G36" s="84">
+      <c r="G35" s="84">
         <v>1626</v>
       </c>
     </row>
-    <row r="38" spans="1:8" ht="16">
-      <c r="A38" s="1"/>
-      <c r="B38" s="86" t="s">
-        <v>37</v>
-      </c>
-      <c r="C38" s="87"/>
-      <c r="D38" s="87"/>
-      <c r="E38" s="87"/>
-      <c r="F38" s="87"/>
-      <c r="G38" s="87"/>
-      <c r="H38" s="87"/>
+    <row r="37" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A37" s="1"/>
+      <c r="B37" s="86" t="s">
+        <v>44</v>
+      </c>
+      <c r="C37" s="87"/>
+      <c r="D37" s="87"/>
+      <c r="E37" s="87"/>
+      <c r="F37" s="87"/>
+      <c r="G37" s="87"/>
+      <c r="H37" s="87"/>
+    </row>
+    <row r="38" spans="1:8" ht="29" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C38" s="104" t="s">
+        <v>45</v>
+      </c>
+      <c r="D38" s="104"/>
+      <c r="E38" s="104"/>
+      <c r="F38" s="104"/>
+      <c r="G38" s="104"/>
+    </row>
+    <row r="39" spans="1:8" ht="31" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C39" s="104" t="s">
+        <v>46</v>
+      </c>
+      <c r="D39" s="104"/>
+      <c r="E39" s="104"/>
+      <c r="F39" s="104"/>
+      <c r="G39" s="104"/>
+    </row>
+    <row r="40" spans="1:8" ht="29" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C40" s="104" t="s">
+        <v>47</v>
+      </c>
+      <c r="D40" s="104"/>
+      <c r="E40" s="104"/>
+      <c r="F40" s="104"/>
+      <c r="G40" s="104"/>
+    </row>
+    <row r="41" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C41" s="105"/>
+      <c r="D41" s="105"/>
+      <c r="E41" s="105"/>
+      <c r="F41" s="105"/>
+      <c r="G41" s="105"/>
     </row>
   </sheetData>
-  <mergeCells count="11">
-    <mergeCell ref="B38:H38"/>
-    <mergeCell ref="B3:G3"/>
-    <mergeCell ref="B8:B18"/>
-    <mergeCell ref="B19:B22"/>
-    <mergeCell ref="B23:B25"/>
-    <mergeCell ref="B26:B32"/>
-    <mergeCell ref="B33:B36"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:C7"/>
+  <mergeCells count="14">
+    <mergeCell ref="C38:G38"/>
+    <mergeCell ref="C39:G39"/>
+    <mergeCell ref="C40:G40"/>
+    <mergeCell ref="B37:H37"/>
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="B7:B17"/>
+    <mergeCell ref="B18:B21"/>
+    <mergeCell ref="B22:B24"/>
+    <mergeCell ref="B25:B31"/>
+    <mergeCell ref="B32:B35"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C5:C6"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="C38" r:id="rId1" xr:uid="{03FDC4C2-9364-5742-AB0B-179167691F19}"/>
+    <hyperlink ref="C39" r:id="rId2" xr:uid="{A92B6CE8-D4FC-8446-9FB5-8260822D9126}"/>
+    <hyperlink ref="C40" r:id="rId3" xr:uid="{1D6E6129-D687-454F-A0AA-16D32B169DDD}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="64" fitToHeight="4" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -1869,11 +1873,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAA77C29-1FFD-6A47-9BFF-0B1C48B5AEA4}">
   <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A29" sqref="A29:A31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="17" customWidth="1"/>
     <col min="2" max="2" width="26.6640625" customWidth="1"/>
@@ -1881,7 +1885,7 @@
     <col min="5" max="6" width="18.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="37" customHeight="1">
+    <row r="1" spans="1:6" ht="37" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -1901,7 +1905,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="17">
+    <row r="2" spans="1:6" ht="17" x14ac:dyDescent="0.15">
       <c r="A2" s="7" t="s">
         <v>0</v>
       </c>
@@ -1912,16 +1916,16 @@
         <v>2023</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E2" s="12">
         <v>2023</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="17">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="17" x14ac:dyDescent="0.15">
       <c r="A3" s="14" t="s">
         <v>4</v>
       </c>
@@ -1941,7 +1945,7 @@
         <v>68524</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="17">
+    <row r="4" spans="1:6" ht="17" x14ac:dyDescent="0.15">
       <c r="A4" s="14" t="s">
         <v>4</v>
       </c>
@@ -1961,7 +1965,7 @@
         <v>17698</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="17">
+    <row r="5" spans="1:6" ht="17" x14ac:dyDescent="0.15">
       <c r="A5" s="14" t="s">
         <v>4</v>
       </c>
@@ -1981,7 +1985,7 @@
         <v>31326</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="34">
+    <row r="6" spans="1:6" ht="34" x14ac:dyDescent="0.15">
       <c r="A6" s="14" t="s">
         <v>4</v>
       </c>
@@ -2001,7 +2005,7 @@
         <v>50322</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="17">
+    <row r="7" spans="1:6" ht="17" x14ac:dyDescent="0.15">
       <c r="A7" s="14" t="s">
         <v>4</v>
       </c>
@@ -2021,7 +2025,7 @@
         <v>24379</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="17">
+    <row r="8" spans="1:6" ht="17" x14ac:dyDescent="0.15">
       <c r="A8" s="14" t="s">
         <v>4</v>
       </c>
@@ -2041,7 +2045,7 @@
         <v>9334</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="34">
+    <row r="9" spans="1:6" ht="34" x14ac:dyDescent="0.15">
       <c r="A9" s="14" t="s">
         <v>4</v>
       </c>
@@ -2061,12 +2065,12 @@
         <v>54306</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="34">
+    <row r="10" spans="1:6" ht="34" x14ac:dyDescent="0.15">
       <c r="A10" s="14" t="s">
         <v>4</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C10" s="20">
         <v>26</v>
@@ -2081,12 +2085,12 @@
         <v>19934</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="34">
+    <row r="11" spans="1:6" ht="34" x14ac:dyDescent="0.15">
       <c r="A11" s="14" t="s">
         <v>4</v>
       </c>
       <c r="B11" s="19" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C11" s="20">
         <v>35</v>
@@ -2101,7 +2105,7 @@
         <v>5236</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="17">
+    <row r="12" spans="1:6" ht="17" x14ac:dyDescent="0.15">
       <c r="A12" s="14" t="s">
         <v>4</v>
       </c>
@@ -2121,7 +2125,7 @@
         <v>12512</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="34">
+    <row r="13" spans="1:6" ht="34" x14ac:dyDescent="0.15">
       <c r="A13" s="14" t="s">
         <v>4</v>
       </c>
@@ -2141,9 +2145,9 @@
         <v>9547</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="34">
+    <row r="14" spans="1:6" ht="34" x14ac:dyDescent="0.15">
       <c r="A14" s="29" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B14" s="30" t="s">
         <v>14</v>
@@ -2161,9 +2165,9 @@
         <v>10967</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="34">
+    <row r="15" spans="1:6" ht="34" x14ac:dyDescent="0.15">
       <c r="A15" s="29" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B15" s="34" t="s">
         <v>15</v>
@@ -2181,9 +2185,9 @@
         <v>11984</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="34">
+    <row r="16" spans="1:6" ht="34" x14ac:dyDescent="0.15">
       <c r="A16" s="29" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B16" s="34" t="s">
         <v>16</v>
@@ -2201,9 +2205,9 @@
         <v>28569</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="34">
+    <row r="17" spans="1:6" ht="34" x14ac:dyDescent="0.15">
       <c r="A17" s="29" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B17" s="40" t="s">
         <v>17</v>
@@ -2221,9 +2225,9 @@
         <v>5339</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="34">
+    <row r="18" spans="1:6" ht="34" x14ac:dyDescent="0.15">
       <c r="A18" s="44" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B18" s="45" t="s">
         <v>19</v>
@@ -2241,9 +2245,9 @@
         <v>18583</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="17">
+    <row r="19" spans="1:6" ht="17" x14ac:dyDescent="0.15">
       <c r="A19" s="44" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B19" s="49" t="s">
         <v>20</v>
@@ -2261,9 +2265,9 @@
         <v>22974</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="17">
+    <row r="20" spans="1:6" ht="17" x14ac:dyDescent="0.15">
       <c r="A20" s="44" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B20" s="53" t="s">
         <v>21</v>
@@ -2281,9 +2285,9 @@
         <v>4701</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="34">
+    <row r="21" spans="1:6" ht="34" x14ac:dyDescent="0.15">
       <c r="A21" s="57" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B21" s="58" t="s">
         <v>23</v>
@@ -2301,9 +2305,9 @@
         <v>8943</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="34">
+    <row r="22" spans="1:6" ht="34" x14ac:dyDescent="0.15">
       <c r="A22" s="57" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B22" s="62" t="s">
         <v>24</v>
@@ -2321,9 +2325,9 @@
         <v>44084</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="17">
+    <row r="23" spans="1:6" ht="17" x14ac:dyDescent="0.15">
       <c r="A23" s="57" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B23" s="62" t="s">
         <v>25</v>
@@ -2341,9 +2345,9 @@
         <v>18583</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="34">
+    <row r="24" spans="1:6" ht="34" x14ac:dyDescent="0.15">
       <c r="A24" s="57" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B24" s="62" t="s">
         <v>26</v>
@@ -2361,12 +2365,12 @@
         <v>12593</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="17">
+    <row r="25" spans="1:6" ht="17" x14ac:dyDescent="0.15">
       <c r="A25" s="57" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B25" s="62" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C25" s="63">
         <v>3</v>
@@ -2381,9 +2385,9 @@
         <v>11460</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="34">
+    <row r="26" spans="1:6" ht="34" x14ac:dyDescent="0.15">
       <c r="A26" s="57" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B26" s="62" t="s">
         <v>27</v>
@@ -2401,9 +2405,9 @@
         <v>16394</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="34">
+    <row r="27" spans="1:6" ht="34" x14ac:dyDescent="0.15">
       <c r="A27" s="57" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B27" s="68" t="s">
         <v>28</v>
@@ -2421,9 +2425,9 @@
         <v>7995</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="17">
+    <row r="28" spans="1:6" ht="17" x14ac:dyDescent="0.15">
       <c r="A28" s="72" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B28" s="73" t="s">
         <v>30</v>
@@ -2441,9 +2445,9 @@
         <v>2454</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="17">
+    <row r="29" spans="1:6" ht="17" x14ac:dyDescent="0.15">
       <c r="A29" s="72" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B29" s="77" t="s">
         <v>31</v>
@@ -2461,9 +2465,9 @@
         <v>3569</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="17">
+    <row r="30" spans="1:6" ht="17" x14ac:dyDescent="0.15">
       <c r="A30" s="72" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B30" s="77" t="s">
         <v>32</v>
@@ -2481,9 +2485,9 @@
         <v>3013</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="17">
+    <row r="31" spans="1:6" ht="17" x14ac:dyDescent="0.15">
       <c r="A31" s="72" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B31" s="81" t="s">
         <v>33</v>
@@ -2502,7 +2506,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="15" type="noConversion"/>
+  <phoneticPr fontId="12" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>